<commit_message>
Clean repo with only relevnt files for preprocessing
</commit_message>
<xml_diff>
--- a/data/IMF ISORA.xlsx
+++ b/data/IMF ISORA.xlsx
@@ -76458,10 +76458,9 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D983349EF0E07A4891C6B05F2378AE33" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="96c552b3d18438292db071d4c8f1afb0">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="29b9448c-835a-49b9-adde-26caac639c00" xmlns:ns3="d7b57de8-4048-43b8-97a9-ce7a87401ded" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="93a54ca3179d3954b437dd8e703ce054" ns2:_="" ns3:_="">
-    <xsd:import namespace="29b9448c-835a-49b9-adde-26caac639c00"/>
-    <xsd:import namespace="d7b57de8-4048-43b8-97a9-ce7a87401ded"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F5E1F8C1127D94A9EF7C9A049B841E7" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="69efe6f401b97f8e817d44789592dc77">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e3d36b8b-345e-449d-8c9a-b7bdc8e37b72" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="56e1b0abd19deea4784b69ac93d516b9" ns2:_="">
+    <xsd:import namespace="e3d36b8b-345e-449d-8c9a-b7bdc8e37b72"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -76472,13 +76471,6 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:Note" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -76486,7 +76478,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="29b9448c-835a-49b9-adde-26caac639c00" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e3d36b8b-345e-449d-8c9a-b7bdc8e37b72" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -76508,57 +76500,6 @@
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Note" ma:index="12" nillable="true" ma:displayName="Note" ma:description="General admin and planning documents" ma:format="Dropdown" ma:internalName="Note">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="14" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="78175662-8596-484a-92c7-351d01561e22" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="19" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d7b57de8-4048-43b8-97a9-ce7a87401ded" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="15" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{b387fd02-f686-4372-a698-03b67302e808}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d7b57de8-4048-43b8-97a9-ce7a87401ded">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -76660,10 +76601,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A57B1C55-6F07-4F41-8F31-9844FB25F764}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CBCDD7-AA4A-4ED9-B6B8-81326E32F59B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9869562-807F-42C3-A71E-D0B1CF3EB352}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4FB8790-CAEB-4D6C-99C9-6ED22C519FC6}"/>
 </file>
</xml_diff>